<commit_message>
feat: added JWT and user logs
</commit_message>
<xml_diff>
--- a/sheet.xlsx
+++ b/sheet.xlsx
@@ -1,53 +1,66 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr/>
-  <workbookProtection/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8d1ee7089cfaf146/Desktop/MDG/bluetooth_door_lock/castle-black/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="3" documentId="11_CA7D508FC464025E63131CF645182E3EC2A78FFC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D41C7480-8B02-445B-A5EF-9B2A0558F237}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="passwords" sheetId="1" r:id="rId1"/>
+    <sheet name="logs" sheetId="2" r:id="rId2"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1" refMode="A1" iterate="0" iterateCount="100" iterateDelta="0.001"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Password Hash</t>
+  </si>
+  <si>
+    <t>orange</t>
+  </si>
+  <si>
+    <t>pbkdf2:sha256:150000$y8rKNCIS$2142ad41d291f6a0d4f95b4125e3796faea57e509b8f90376c57efa72736f191</t>
+  </si>
+  <si>
+    <t>sickaada</t>
+  </si>
+  <si>
+    <t>pbkdf2:sha256:150000$QEa2sjpJ$f788d0f18c02d522266a2ea851a2b31b07f67e3e41b12871941046c4e1ec5ad9</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <sz val="10"/>
     </font>
     <font>
-      <name val="Arial"/>
-      <family val="0"/>
+      <b/>
       <sz val="10"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <family val="0"/>
-      <sz val="10"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <family val="0"/>
-      <sz val="10"/>
-    </font>
-    <font>
       <name val="Arial"/>
       <family val="2"/>
-      <b val="1"/>
-      <sz val="10"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -62,107 +75,27 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="6">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1">
-      <alignment horizontal="general" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom"/>
-    </xf>
+  <cellXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="1" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="2" builtinId="6"/>
-    <cellStyle name="Currency" xfId="3" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
-    <cellStyle name="Percent" xfId="5" builtinId="5"/>
   </cellStyles>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -450,69 +383,60 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr filterMode="0">
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr fitToPage="0"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col width="14.9" customWidth="1" style="2" min="2" max="2"/>
+    <col min="2" max="2" width="14.90625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="12.8" customHeight="1" s="3">
-      <c r="A1" s="4" t="inlineStr">
-        <is>
-          <t>Username</t>
-        </is>
-      </c>
-      <c r="B1" s="4" t="inlineStr">
-        <is>
-          <t>Password Hash</t>
-        </is>
+    <row r="1" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
       </c>
     </row>
-    <row r="2" ht="12.8" customHeight="1" s="3">
-      <c r="A2" s="2" t="inlineStr">
-        <is>
-          <t>orange</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>pbkdf2:sha256:150000$y8rKNCIS$2142ad41d291f6a0d4f95b4125e3796faea57e509b8f90376c57efa72736f191</t>
-        </is>
+    <row r="2" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
       </c>
     </row>
-    <row r="3" ht="12.8" customHeight="1" s="3">
-      <c r="A3" s="2" t="inlineStr">
-        <is>
-          <t>sickaada</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>pbkdf2:sha256:150000$QEa2sjpJ$f788d0f18c02d522266a2ea851a2b31b07f67e3e41b12871941046c4e1ec5ad9</t>
-        </is>
+    <row r="3" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
-  <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup orientation="portrait" paperSize="9" scale="100" fitToHeight="1" fitToWidth="1" firstPageNumber="1" useFirstPageNumber="1" pageOrder="downThenOver" blackAndWhite="0" draft="0" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentOddEven="0" differentFirst="0">
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12 &amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12 Page &amp;P</oddFooter>
-    <evenHeader/>
-    <evenFooter/>
-    <firstHeader/>
-    <firstFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C407DA5D-2960-4CF9-9139-C886B756FA0D}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>